<commit_message>
Use openpyxl for getting row/col bounds and update the syntax to use type in line hinting
</commit_message>
<xml_diff>
--- a/Tests/Example.xlsx
+++ b/Tests/Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\PycharmProjects\xslxObject\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9800037F-FE2B-4C89-BDFD-2C221E2765B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E96DE2-D4CB-4532-8F0A-14A9E564A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A607A3D5-49F7-4608-ACA3-EE39EC8A6043}"/>
+    <workbookView xWindow="37320" yWindow="1020" windowWidth="17025" windowHeight="10950" xr2:uid="{A607A3D5-49F7-4608-ACA3-EE39EC8A6043}"/>
   </bookViews>
   <sheets>
     <sheet name="Deaths" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>A38 Scarlet fever</t>
+  </si>
+  <si>
+    <t>A34</t>
+  </si>
+  <si>
+    <t>B31</t>
+  </si>
+  <si>
+    <t>G564</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A79D4B-362A-4794-A53A-CC65F0FC9E03}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +572,30 @@
       </c>
       <c r="B12" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>